<commit_message>
Normaliseerde database design aangepast
</commit_message>
<xml_diff>
--- a/3. Construction_Phase/Normalised_Database_Design/Normalised_Database_Design.xlsx
+++ b/3. Construction_Phase/Normalised_Database_Design/Normalised_Database_Design.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Project_P5\3. Construction_Phase\Genormaliseerd Databaseontwerp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Project_P5\3. Construction_Phase\Normalised_Database_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>tbl_customers</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Department</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -241,11 +244,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -858,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AH23"/>
+  <dimension ref="A2:AG23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +874,7 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
@@ -901,12 +905,12 @@
     <col min="34" max="34" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1006,16 +1010,13 @@
       <c r="AG3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AH3" s="2" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1031,13 +1032,16 @@
       <c r="H8" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="I8" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1054,12 +1058,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
@@ -1072,13 +1076,16 @@
       <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>

</xml_diff>